<commit_message>
update function CRUD Account
</commit_message>
<xml_diff>
--- a/sources/hsts-demo/src/main/resources/static/Template.xlsx
+++ b/sources/hsts-demo/src/main/resources/static/Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Email</t>
   </si>
@@ -37,38 +37,6 @@
     <t>ROLE</t>
   </si>
   <si>
-    <r>
-      <t>Gender</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ROLE</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
     <t>MALE</t>
   </si>
   <si>
@@ -94,31 +62,13 @@
   </si>
   <si>
     <t>&lt;- DO NOT DELETE</t>
-  </si>
-  <si>
-    <t>khuonghcm1@gmail.com</t>
-  </si>
-  <si>
-    <t>31-11-1994</t>
-  </si>
-  <si>
-    <t>22-12-1993</t>
-  </si>
-  <si>
-    <t>Vuong Di</t>
-  </si>
-  <si>
-    <t>Ha Kim Quy</t>
-  </si>
-  <si>
-    <t>khuonghcm3@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,14 +88,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -600,7 +542,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +555,7 @@
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -626,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>3</v>
@@ -648,7 +591,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
@@ -657,71 +600,51 @@
         <v>1</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K2" s="10">
         <v>1</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="12">
-        <v>3</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="12"/>
       <c r="H3" s="10">
         <v>2</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K3" s="10">
         <v>2</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="12"/>
       <c r="K4" s="10">
         <v>3</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -734,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -742,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -752,10 +675,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>